<commit_message>
Backup QR Scanner data - 2025-11-19T07:05:49.110Z - Cache Bust: 1763535949110
</commit_message>
<xml_diff>
--- a/log_history/Y2_B2526_Parasitology_SGD_POS_scanner1763533479392_f71e38082cd54d27436e85b09564b917f0cd2df53e3050bee655eeab2adc060c.xlsx
+++ b/log_history/Y2_B2526_Parasitology_SGD_POS_scanner1763533479392_f71e38082cd54d27436e85b09564b917f0cd2df53e3050bee655eeab2adc060c.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Session" sheetId="1" r:id="rId1"/>
+    <sheet name="Parasitology_SGD_POS" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:F55"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1422,9 +1422,89 @@
         <v>Alshimaa_khaled@med.asu.edu.eg</v>
       </c>
     </row>
+    <row r="52">
+      <c r="A52" t="str">
+        <v>244632</v>
+      </c>
+      <c r="B52" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C52" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D52" t="str">
+        <v>09:02:26</v>
+      </c>
+      <c r="E52" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F52" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v>244631</v>
+      </c>
+      <c r="B53" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C53" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D53" t="str">
+        <v>09:02:32</v>
+      </c>
+      <c r="E53" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F53" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="str">
+        <v>244571</v>
+      </c>
+      <c r="B54" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C54" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D54" t="str">
+        <v>09:03:01</v>
+      </c>
+      <c r="E54" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F54" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="str">
+        <v>244499</v>
+      </c>
+      <c r="B55" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C55" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D55" t="str">
+        <v>09:03:10</v>
+      </c>
+      <c r="E55" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F55" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F51"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F55"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Backup QR Scanner data - 2025-11-19T07:32:34.593Z - Cache Bust: 1763537554593
</commit_message>
<xml_diff>
--- a/log_history/Y2_B2526_Parasitology_SGD_POS_scanner1763533479392_f71e38082cd54d27436e85b09564b917f0cd2df53e3050bee655eeab2adc060c.xlsx
+++ b/log_history/Y2_B2526_Parasitology_SGD_POS_scanner1763533479392_f71e38082cd54d27436e85b09564b917f0cd2df53e3050bee655eeab2adc060c.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Session" sheetId="1" r:id="rId1"/>
+    <sheet name="Parasitology_SGD_POS" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F55"/>
+  <dimension ref="A1:F143"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1502,9 +1502,1769 @@
         <v>Alshimaa_khaled@med.asu.edu.eg</v>
       </c>
     </row>
+    <row r="56">
+      <c r="A56" t="str">
+        <v>241353</v>
+      </c>
+      <c r="B56" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C56" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D56" t="str">
+        <v>09:14:15</v>
+      </c>
+      <c r="E56" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F56" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="str">
+        <v>241240</v>
+      </c>
+      <c r="B57" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C57" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D57" t="str">
+        <v>09:14:32</v>
+      </c>
+      <c r="E57" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F57" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="str">
+        <v>241466</v>
+      </c>
+      <c r="B58" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C58" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D58" t="str">
+        <v>09:14:50</v>
+      </c>
+      <c r="E58" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F58" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="str">
+        <v>244348</v>
+      </c>
+      <c r="B59" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C59" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D59" t="str">
+        <v>09:15:03</v>
+      </c>
+      <c r="E59" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F59" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="str">
+        <v>241340</v>
+      </c>
+      <c r="B60" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C60" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D60" t="str">
+        <v>09:15:17</v>
+      </c>
+      <c r="E60" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F60" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="str">
+        <v>241350</v>
+      </c>
+      <c r="B61" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C61" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D61" t="str">
+        <v>09:15:30</v>
+      </c>
+      <c r="E61" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F61" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="str">
+        <v>241388</v>
+      </c>
+      <c r="B62" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C62" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D62" t="str">
+        <v>09:17:29</v>
+      </c>
+      <c r="E62" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F62" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="str">
+        <v>241393</v>
+      </c>
+      <c r="B63" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C63" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D63" t="str">
+        <v>09:17:46</v>
+      </c>
+      <c r="E63" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F63" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="str">
+        <v>241241</v>
+      </c>
+      <c r="B64" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C64" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D64" t="str">
+        <v>09:17:55</v>
+      </c>
+      <c r="E64" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F64" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="str">
+        <v>241281</v>
+      </c>
+      <c r="B65" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C65" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D65" t="str">
+        <v>09:18:06</v>
+      </c>
+      <c r="E65" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F65" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="str">
+        <v>241284</v>
+      </c>
+      <c r="B66" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C66" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D66" t="str">
+        <v>09:18:33</v>
+      </c>
+      <c r="E66" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F66" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="str">
+        <v>241280</v>
+      </c>
+      <c r="B67" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C67" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D67" t="str">
+        <v>09:18:43</v>
+      </c>
+      <c r="E67" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F67" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="str">
+        <v>241394</v>
+      </c>
+      <c r="B68" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C68" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D68" t="str">
+        <v>09:18:55</v>
+      </c>
+      <c r="E68" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F68" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="str">
+        <v>241314</v>
+      </c>
+      <c r="B69" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C69" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D69" t="str">
+        <v>09:19:08</v>
+      </c>
+      <c r="E69" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F69" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="str">
+        <v>241266</v>
+      </c>
+      <c r="B70" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C70" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D70" t="str">
+        <v>09:19:20</v>
+      </c>
+      <c r="E70" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F70" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="str">
+        <v>241245</v>
+      </c>
+      <c r="B71" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C71" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D71" t="str">
+        <v>09:19:31</v>
+      </c>
+      <c r="E71" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F71" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="str">
+        <v>244391</v>
+      </c>
+      <c r="B72" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C72" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D72" t="str">
+        <v>09:19:42</v>
+      </c>
+      <c r="E72" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F72" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="str">
+        <v>241278</v>
+      </c>
+      <c r="B73" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C73" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D73" t="str">
+        <v>09:19:57</v>
+      </c>
+      <c r="E73" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F73" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="str">
+        <v>241472</v>
+      </c>
+      <c r="B74" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C74" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D74" t="str">
+        <v>09:20:12</v>
+      </c>
+      <c r="E74" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F74" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="str">
+        <v>241420</v>
+      </c>
+      <c r="B75" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C75" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D75" t="str">
+        <v>09:20:26</v>
+      </c>
+      <c r="E75" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F75" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="str">
+        <v>241355</v>
+      </c>
+      <c r="B76" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C76" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D76" t="str">
+        <v>09:20:44</v>
+      </c>
+      <c r="E76" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F76" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="str">
+        <v>241305</v>
+      </c>
+      <c r="B77" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C77" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D77" t="str">
+        <v>09:20:56</v>
+      </c>
+      <c r="E77" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F77" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="str">
+        <v>241276</v>
+      </c>
+      <c r="B78" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C78" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D78" t="str">
+        <v>09:21:10</v>
+      </c>
+      <c r="E78" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F78" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="str">
+        <v>241478</v>
+      </c>
+      <c r="B79" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C79" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D79" t="str">
+        <v>09:21:23</v>
+      </c>
+      <c r="E79" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F79" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="str">
+        <v>244256</v>
+      </c>
+      <c r="B80" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C80" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D80" t="str">
+        <v>09:21:35</v>
+      </c>
+      <c r="E80" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F80" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="str">
+        <v>241318</v>
+      </c>
+      <c r="B81" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C81" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D81" t="str">
+        <v>09:21:59</v>
+      </c>
+      <c r="E81" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F81" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="str">
+        <v>241410</v>
+      </c>
+      <c r="B82" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C82" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D82" t="str">
+        <v>09:22:16</v>
+      </c>
+      <c r="E82" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F82" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="str">
+        <v>241277</v>
+      </c>
+      <c r="B83" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C83" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D83" t="str">
+        <v>09:22:35</v>
+      </c>
+      <c r="E83" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F83" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="str">
+        <v>241374</v>
+      </c>
+      <c r="B84" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C84" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D84" t="str">
+        <v>09:22:52</v>
+      </c>
+      <c r="E84" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F84" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="str">
+        <v>241297</v>
+      </c>
+      <c r="B85" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C85" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D85" t="str">
+        <v>09:24:14</v>
+      </c>
+      <c r="E85" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F85" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="str">
+        <v>241298</v>
+      </c>
+      <c r="B86" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C86" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D86" t="str">
+        <v>09:24:20</v>
+      </c>
+      <c r="E86" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F86" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="str">
+        <v>241417</v>
+      </c>
+      <c r="B87" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C87" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D87" t="str">
+        <v>09:24:23</v>
+      </c>
+      <c r="E87" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F87" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="str">
+        <v>241367</v>
+      </c>
+      <c r="B88" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C88" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D88" t="str">
+        <v>09:24:28</v>
+      </c>
+      <c r="E88" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F88" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="str">
+        <v>241378</v>
+      </c>
+      <c r="B89" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C89" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D89" t="str">
+        <v>09:24:49</v>
+      </c>
+      <c r="E89" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F89" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="str">
+        <v>241409</v>
+      </c>
+      <c r="B90" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C90" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D90" t="str">
+        <v>09:24:55</v>
+      </c>
+      <c r="E90" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F90" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="str">
+        <v>241413</v>
+      </c>
+      <c r="B91" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C91" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D91" t="str">
+        <v>09:24:59</v>
+      </c>
+      <c r="E91" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F91" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="str">
+        <v>241464</v>
+      </c>
+      <c r="B92" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C92" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D92" t="str">
+        <v>09:25:04</v>
+      </c>
+      <c r="E92" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F92" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="str">
+        <v>241376</v>
+      </c>
+      <c r="B93" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C93" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D93" t="str">
+        <v>09:25:08</v>
+      </c>
+      <c r="E93" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F93" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="str">
+        <v>241473</v>
+      </c>
+      <c r="B94" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C94" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D94" t="str">
+        <v>09:25:14</v>
+      </c>
+      <c r="E94" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F94" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="str">
+        <v>241465</v>
+      </c>
+      <c r="B95" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C95" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D95" t="str">
+        <v>09:25:21</v>
+      </c>
+      <c r="E95" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F95" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="str">
+        <v>241359</v>
+      </c>
+      <c r="B96" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C96" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D96" t="str">
+        <v>09:25:26</v>
+      </c>
+      <c r="E96" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F96" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="str">
+        <v>241386</v>
+      </c>
+      <c r="B97" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C97" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D97" t="str">
+        <v>09:25:30</v>
+      </c>
+      <c r="E97" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F97" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="str">
+        <v>241412</v>
+      </c>
+      <c r="B98" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C98" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D98" t="str">
+        <v>09:25:34</v>
+      </c>
+      <c r="E98" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F98" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="str">
+        <v>241425</v>
+      </c>
+      <c r="B99" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C99" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D99" t="str">
+        <v>09:25:39</v>
+      </c>
+      <c r="E99" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F99" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="str">
+        <v>241427</v>
+      </c>
+      <c r="B100" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C100" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D100" t="str">
+        <v>09:25:44</v>
+      </c>
+      <c r="E100" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F100" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="str">
+        <v>241433</v>
+      </c>
+      <c r="B101" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C101" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D101" t="str">
+        <v>09:25:49</v>
+      </c>
+      <c r="E101" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F101" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="str">
+        <v>241442</v>
+      </c>
+      <c r="B102" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C102" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D102" t="str">
+        <v>09:25:53</v>
+      </c>
+      <c r="E102" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F102" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="str">
+        <v>241436</v>
+      </c>
+      <c r="B103" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C103" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D103" t="str">
+        <v>09:25:57</v>
+      </c>
+      <c r="E103" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F103" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="str">
+        <v>241290</v>
+      </c>
+      <c r="B104" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C104" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D104" t="str">
+        <v>09:26:01</v>
+      </c>
+      <c r="E104" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F104" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="str">
+        <v>241265</v>
+      </c>
+      <c r="B105" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C105" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D105" t="str">
+        <v>09:26:09</v>
+      </c>
+      <c r="E105" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F105" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="str">
+        <v>241468</v>
+      </c>
+      <c r="B106" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C106" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D106" t="str">
+        <v>09:26:13</v>
+      </c>
+      <c r="E106" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F106" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="str">
+        <v>241299</v>
+      </c>
+      <c r="B107" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C107" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D107" t="str">
+        <v>09:26:17</v>
+      </c>
+      <c r="E107" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F107" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="str">
+        <v>241279</v>
+      </c>
+      <c r="B108" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C108" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D108" t="str">
+        <v>09:26:23</v>
+      </c>
+      <c r="E108" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F108" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="str">
+        <v>241295</v>
+      </c>
+      <c r="B109" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C109" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D109" t="str">
+        <v>09:26:28</v>
+      </c>
+      <c r="E109" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F109" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="str">
+        <v>241283</v>
+      </c>
+      <c r="B110" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C110" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D110" t="str">
+        <v>09:26:32</v>
+      </c>
+      <c r="E110" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F110" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="str">
+        <v>241469</v>
+      </c>
+      <c r="B111" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C111" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D111" t="str">
+        <v>09:26:33</v>
+      </c>
+      <c r="E111" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F111" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="str">
+        <v>241252</v>
+      </c>
+      <c r="B112" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C112" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D112" t="str">
+        <v>09:26:42</v>
+      </c>
+      <c r="E112" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F112" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="str">
+        <v>241426</v>
+      </c>
+      <c r="B113" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C113" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D113" t="str">
+        <v>09:26:46</v>
+      </c>
+      <c r="E113" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F113" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="str">
+        <v>241397</v>
+      </c>
+      <c r="B114" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C114" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D114" t="str">
+        <v>09:26:49</v>
+      </c>
+      <c r="E114" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F114" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="str">
+        <v>241405</v>
+      </c>
+      <c r="B115" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C115" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D115" t="str">
+        <v>09:26:55</v>
+      </c>
+      <c r="E115" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F115" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="str">
+        <v>241482</v>
+      </c>
+      <c r="B116" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C116" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D116" t="str">
+        <v>09:26:59</v>
+      </c>
+      <c r="E116" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F116" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="str">
+        <v>241432</v>
+      </c>
+      <c r="B117" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C117" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D117" t="str">
+        <v>09:27:04</v>
+      </c>
+      <c r="E117" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F117" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="str">
+        <v>241450</v>
+      </c>
+      <c r="B118" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C118" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D118" t="str">
+        <v>09:27:08</v>
+      </c>
+      <c r="E118" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F118" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="str">
+        <v>241254</v>
+      </c>
+      <c r="B119" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C119" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D119" t="str">
+        <v>09:27:13</v>
+      </c>
+      <c r="E119" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F119" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="str">
+        <v>241480</v>
+      </c>
+      <c r="B120" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C120" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D120" t="str">
+        <v>09:27:26</v>
+      </c>
+      <c r="E120" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F120" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="str">
+        <v>241321</v>
+      </c>
+      <c r="B121" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C121" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D121" t="str">
+        <v>09:27:31</v>
+      </c>
+      <c r="E121" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F121" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="str">
+        <v>241322</v>
+      </c>
+      <c r="B122" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C122" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D122" t="str">
+        <v>09:27:36</v>
+      </c>
+      <c r="E122" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F122" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="str">
+        <v>241444</v>
+      </c>
+      <c r="B123" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C123" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D123" t="str">
+        <v>09:27:40</v>
+      </c>
+      <c r="E123" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F123" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="str">
+        <v>241370</v>
+      </c>
+      <c r="B124" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C124" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D124" t="str">
+        <v>09:27:45</v>
+      </c>
+      <c r="E124" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F124" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="str">
+        <v>241439</v>
+      </c>
+      <c r="B125" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C125" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D125" t="str">
+        <v>09:27:51</v>
+      </c>
+      <c r="E125" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F125" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="str">
+        <v>241244</v>
+      </c>
+      <c r="B126" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C126" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D126" t="str">
+        <v>09:28:00</v>
+      </c>
+      <c r="E126" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F126" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="str">
+        <v>241387</v>
+      </c>
+      <c r="B127" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C127" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D127" t="str">
+        <v>09:28:02</v>
+      </c>
+      <c r="E127" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F127" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="str">
+        <v>241476</v>
+      </c>
+      <c r="B128" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C128" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D128" t="str">
+        <v>09:28:09</v>
+      </c>
+      <c r="E128" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F128" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="str">
+        <v>241475</v>
+      </c>
+      <c r="B129" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C129" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D129" t="str">
+        <v>09:28:17</v>
+      </c>
+      <c r="E129" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F129" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="str">
+        <v>241301</v>
+      </c>
+      <c r="B130" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C130" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D130" t="str">
+        <v>09:28:18</v>
+      </c>
+      <c r="E130" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F130" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="str">
+        <v>241403</v>
+      </c>
+      <c r="B131" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C131" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D131" t="str">
+        <v>09:28:24</v>
+      </c>
+      <c r="E131" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F131" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="str">
+        <v>241291</v>
+      </c>
+      <c r="B132" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C132" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D132" t="str">
+        <v>09:28:35</v>
+      </c>
+      <c r="E132" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F132" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="str">
+        <v>241315</v>
+      </c>
+      <c r="B133" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C133" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D133" t="str">
+        <v>09:28:39</v>
+      </c>
+      <c r="E133" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F133" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="str">
+        <v>241342</v>
+      </c>
+      <c r="B134" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C134" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D134" t="str">
+        <v>09:29:13</v>
+      </c>
+      <c r="E134" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F134" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="str">
+        <v>241268</v>
+      </c>
+      <c r="B135" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C135" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D135" t="str">
+        <v>09:29:17</v>
+      </c>
+      <c r="E135" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F135" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="str">
+        <v>241259</v>
+      </c>
+      <c r="B136" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C136" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D136" t="str">
+        <v>09:29:22</v>
+      </c>
+      <c r="E136" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F136" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="str">
+        <v>241303</v>
+      </c>
+      <c r="B137" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C137" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D137" t="str">
+        <v>09:29:28</v>
+      </c>
+      <c r="E137" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F137" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="str">
+        <v>241296</v>
+      </c>
+      <c r="B138" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C138" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D138" t="str">
+        <v>09:29:33</v>
+      </c>
+      <c r="E138" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F138" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="str">
+        <v>241286</v>
+      </c>
+      <c r="B139" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C139" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D139" t="str">
+        <v>09:29:38</v>
+      </c>
+      <c r="E139" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F139" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="str">
+        <v>241431</v>
+      </c>
+      <c r="B140" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C140" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D140" t="str">
+        <v>09:29:43</v>
+      </c>
+      <c r="E140" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F140" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="str">
+        <v>241289</v>
+      </c>
+      <c r="B141" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C141" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D141" t="str">
+        <v>09:29:48</v>
+      </c>
+      <c r="E141" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F141" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="str">
+        <v>241300</v>
+      </c>
+      <c r="B142" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C142" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D142" t="str">
+        <v>09:29:52</v>
+      </c>
+      <c r="E142" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F142" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="str">
+        <v>241122</v>
+      </c>
+      <c r="B143" t="str">
+        <v>Parasitology SGD/POS</v>
+      </c>
+      <c r="C143" t="str">
+        <v>19/11/2025</v>
+      </c>
+      <c r="D143" t="str">
+        <v>09:29:55</v>
+      </c>
+      <c r="E143" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F143" t="str">
+        <v>Alshimaa_khaled@med.asu.edu.eg</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F55"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F143"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>